<commit_message>
reorders columns in recapture and release tables and updates metadata to match
</commit_message>
<xml_diff>
--- a/data-raw/metadata/recapture-metadata.xlsx
+++ b/data-raw/metadata/recapture-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE3D6AB-38CC-F64D-A566-C3ED6A5BD5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13DC27D-4307-D747-87FE-D6A2EF35C803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -143,12 +143,6 @@
   </si>
   <si>
     <t>YYYY-MM-DD</t>
-  </si>
-  <si>
-    <t>subsite</t>
-  </si>
-  <si>
-    <t>Subsite for release.</t>
   </si>
   <si>
     <t>Site where fish were released. Levels =c("VB", "CCRB", "P4", NA)</t>
@@ -599,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,10 +657,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -677,32 +671,39 @@
       <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -713,32 +714,25 @@
       <c r="E4" t="s">
         <v>23</v>
       </c>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -805,38 +799,21 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G11" s="6"/>
+    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G10" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1022" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1022" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1022" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
standardizes release sites in recapture and release and adds placeholder columns
</commit_message>
<xml_diff>
--- a/data-raw/metadata/recapture-metadata.xlsx
+++ b/data-raw/metadata/recapture-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13DC27D-4307-D747-87FE-D6A2EF35C803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B905B31A-DCA7-5C41-8ED9-A00739232247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -130,9 +130,6 @@
     <t>ordinal</t>
   </si>
   <si>
-    <t>Site where recapture samples were taken. Levels = c("Clear Creek", "Upper Battle Creek")</t>
-  </si>
-  <si>
     <t>Key to link with recapture table</t>
   </si>
   <si>
@@ -145,10 +142,25 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>Site where fish were released. Levels =c("VB", "CCRB", "P4", NA)</t>
-  </si>
-  <si>
     <t>2003-12-04</t>
+  </si>
+  <si>
+    <t>Site where fish were released. Levels = c("vulture bar", "clear creek road bridge", "grand matthews permanent turbidity monitoring site", NA)</t>
+  </si>
+  <si>
+    <t>Site where recapture samples were taken. Levels = c("lower clear creek", "upper clear creek", "upper battle creek")</t>
+  </si>
+  <si>
+    <t>fws_run</t>
+  </si>
+  <si>
+    <t>hatchery_origin</t>
+  </si>
+  <si>
+    <t>FWS identified run of fish recaptured</t>
+  </si>
+  <si>
+    <t>Origin of hatchery fish</t>
   </si>
 </sst>
 </file>
@@ -596,7 +608,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,13 +672,13 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -683,16 +695,16 @@
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>31</v>
@@ -700,7 +712,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
@@ -709,7 +721,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -721,13 +733,13 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -745,7 +757,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -778,7 +790,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
         <v>26</v>
@@ -799,7 +811,40 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G10" s="6"/>
     </row>

</xml_diff>

<commit_message>
fixes issues for upload
</commit_message>
<xml_diff>
--- a/data-raw/metadata/recapture-metadata.xlsx
+++ b/data-raw/metadata/recapture-metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20981CAA-BACB-A346-A916-12A6584952BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F90FBB-0A88-394F-9EFB-25E7A840945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29980" yWindow="1780" windowWidth="32860" windowHeight="20060" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -146,18 +146,6 @@
   </si>
   <si>
     <t>Site where recapture samples were taken. Levels = c("lower clear creek", "upper clear creek", "upper battle creek")</t>
-  </si>
-  <si>
-    <t>fws_run</t>
-  </si>
-  <si>
-    <t>hatchery_origin</t>
-  </si>
-  <si>
-    <t>FWS identified run of fish recaptured</t>
-  </si>
-  <si>
-    <t>Origin of hatchery fish</t>
   </si>
   <si>
     <t>2024-04-07</t>
@@ -605,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,7 +695,7 @@
         <v>37</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -812,53 +800,19 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G10" s="6"/>
+      <c r="G8" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1019" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1019" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1019" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>